<commit_message>
This commit will break stuff
</commit_message>
<xml_diff>
--- a/test_thing.xlsx
+++ b/test_thing.xlsx
@@ -1,10 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24026"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CDED145B-4A8E-405F-A07C-ADA97402780B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -14,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="7">
   <si>
     <t>etse</t>
   </si>
@@ -23,12 +24,24 @@
   </si>
   <si>
     <t>gabe</t>
+  </si>
+  <si>
+    <t>not gabe</t>
+  </si>
+  <si>
+    <t>train</t>
+  </si>
+  <si>
+    <t>etse2</t>
+  </si>
+  <si>
+    <t>etse3</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -153,6 +166,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -188,6 +218,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -363,21 +410,29 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E23" sqref="E23"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B5" t="s">
         <v>2</v>
       </c>
@@ -388,20 +443,31 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D6" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>1</v>
       </c>
       <c r="B14" t="s">
         <v>2</v>
       </c>
+      <c r="C14" t="s">
+        <v>3</v>
+      </c>
       <c r="D14" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="C16" t="b">
         <v>1</v>
+      </c>
+      <c r="D16" t="b">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>